<commit_message>
Added changes due to Daylight savings time.
Added in green row shading if event is active.
</commit_message>
<xml_diff>
--- a/DI_Timer_App/Immortal_Lookup_Table.xlsx
+++ b/DI_Timer_App/Immortal_Lookup_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\diablo_immortal_event_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4EC1BA-BFE6-41F0-B4C3-4F159EDEA742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4363B9AF-9CA1-4705-8C3A-F84EA2B5D842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30675" yWindow="930" windowWidth="21600" windowHeight="11385" xr2:uid="{F68A42B3-28CA-4941-B9AB-48F8CCD3EE7B}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{F68A42B3-28CA-4941-B9AB-48F8CCD3EE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,28 +52,28 @@
     <t>Active?</t>
   </si>
   <si>
-    <t>Battlegrounds 8AM</t>
-  </si>
-  <si>
-    <t>Battlegrounds 12PM</t>
-  </si>
-  <si>
-    <t>Battlegrounds 6PM</t>
-  </si>
-  <si>
-    <t>Battlegrounds 10PM</t>
-  </si>
-  <si>
-    <t>Rite of Exile 8PM</t>
-  </si>
-  <si>
-    <t>Defend the Vault 12PM</t>
-  </si>
-  <si>
-    <t>Defend the Vault 7PM</t>
-  </si>
-  <si>
-    <t>Corvus Expedition 830PM</t>
+    <t>Defend the Vault 1</t>
+  </si>
+  <si>
+    <t>Defend the Vault 2</t>
+  </si>
+  <si>
+    <t>Battlegrounds 1</t>
+  </si>
+  <si>
+    <t>Battlegrounds 2</t>
+  </si>
+  <si>
+    <t>Battlegrounds 3</t>
+  </si>
+  <si>
+    <t>Battlegrounds 4</t>
+  </si>
+  <si>
+    <t>Corvus Expedition</t>
+  </si>
+  <si>
+    <t>Rite of Exile</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,42 +457,42 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>